<commit_message>
MML-23: Corridas en LAM con patch para venezuela en GNPXC
</commit_message>
<xml_diff>
--- a/notebooks/data/output/diff_porcentual_LAM.xlsx
+++ b/notebooks/data/output/diff_porcentual_LAM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>POP</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>GNPXC</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -460,6 +465,9 @@
       <c r="C2" t="n">
         <v>-3.815155047135888</v>
       </c>
+      <c r="D2" t="n">
+        <v>-21.7285019360561</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -471,6 +479,9 @@
       <c r="C3" t="n">
         <v>-3.617706034003404</v>
       </c>
+      <c r="D3" t="n">
+        <v>-25.08060966185799</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -482,6 +493,9 @@
       <c r="C4" t="n">
         <v>-3.295588763929543</v>
       </c>
+      <c r="D4" t="n">
+        <v>-27.10010129686633</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -493,6 +507,9 @@
       <c r="C5" t="n">
         <v>-2.871311375045916</v>
       </c>
+      <c r="D5" t="n">
+        <v>-27.06908960397979</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -504,6 +521,9 @@
       <c r="C6" t="n">
         <v>-2.352886144634671</v>
       </c>
+      <c r="D6" t="n">
+        <v>-28.8825220754527</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -515,6 +535,9 @@
       <c r="C7" t="n">
         <v>-1.743734241260364</v>
       </c>
+      <c r="D7" t="n">
+        <v>-29.94859058006045</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -526,6 +549,9 @@
       <c r="C8" t="n">
         <v>-1.120156666764762</v>
       </c>
+      <c r="D8" t="n">
+        <v>-25.89324583683593</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -537,6 +563,9 @@
       <c r="C9" t="n">
         <v>-0.4222568049491471</v>
       </c>
+      <c r="D9" t="n">
+        <v>-19.93608370400428</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -548,6 +577,9 @@
       <c r="C10" t="n">
         <v>0.3684442398899344</v>
       </c>
+      <c r="D10" t="n">
+        <v>-16.82127840733422</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -559,6 +591,9 @@
       <c r="C11" t="n">
         <v>1.230769230769231</v>
       </c>
+      <c r="D11" t="n">
+        <v>-12.86973756267729</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -570,6 +605,9 @@
       <c r="C12" t="n">
         <v>2.11082215166648</v>
       </c>
+      <c r="D12" t="n">
+        <v>-8.211208407277148</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -581,6 +619,9 @@
       <c r="C13" t="n">
         <v>2.977468459579256</v>
       </c>
+      <c r="D13" t="n">
+        <v>-7.566958904969685</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -592,6 +633,9 @@
       <c r="C14" t="n">
         <v>3.80174969179877</v>
       </c>
+      <c r="D14" t="n">
+        <v>-6.956106265842839</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -603,6 +647,9 @@
       <c r="C15" t="n">
         <v>4.610926166893115</v>
       </c>
+      <c r="D15" t="n">
+        <v>-4.780545139431</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -614,6 +661,9 @@
       <c r="C16" t="n">
         <v>5.341240389625369</v>
       </c>
+      <c r="D16" t="n">
+        <v>-5.055153423506624</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -625,6 +675,9 @@
       <c r="C17" t="n">
         <v>6.073857833228109</v>
       </c>
+      <c r="D17" t="n">
+        <v>0.4800652948802238</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -636,6 +689,9 @@
       <c r="C18" t="n">
         <v>6.51405474645861</v>
       </c>
+      <c r="D18" t="n">
+        <v>12.27015730682708</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -647,6 +703,9 @@
       <c r="C19" t="n">
         <v>6.853049611651373</v>
       </c>
+      <c r="D19" t="n">
+        <v>18.24331659142144</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -658,6 +717,9 @@
       <c r="C20" t="n">
         <v>7.105407699605533</v>
       </c>
+      <c r="D20" t="n">
+        <v>21.94851821104215</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -669,6 +731,9 @@
       <c r="C21" t="n">
         <v>7.163226129534832</v>
       </c>
+      <c r="D21" t="n">
+        <v>26.64014873022778</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -680,6 +745,9 @@
       <c r="C22" t="n">
         <v>6.993608548629833</v>
       </c>
+      <c r="D22" t="n">
+        <v>38.03504935997214</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -691,6 +759,9 @@
       <c r="C23" t="n">
         <v>6.847839595675048</v>
       </c>
+      <c r="D23" t="n">
+        <v>45.68189272286769</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -702,6 +773,9 @@
       <c r="C24" t="n">
         <v>6.723516756952905</v>
       </c>
+      <c r="D24" t="n">
+        <v>56.21589622837237</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -713,6 +787,9 @@
       <c r="C25" t="n">
         <v>6.661635108437479</v>
       </c>
+      <c r="D25" t="n">
+        <v>70.5583284097419</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -723,6 +800,9 @@
       </c>
       <c r="C26" t="n">
         <v>6.667453918572257</v>
+      </c>
+      <c r="D26" t="n">
+        <v>84.2374238461634</v>
       </c>
     </row>
   </sheetData>

</xml_diff>